<commit_message>
update fetchUser and mailing-list
</commit_message>
<xml_diff>
--- a/public/contact_group_2.xlsx
+++ b/public/contact_group_2.xlsx
@@ -115,15 +115,6 @@
     <t>380995111333</t>
   </si>
   <si>
-    <t>333333333333</t>
-  </si>
-  <si>
-    <t>444444444444</t>
-  </si>
-  <si>
-    <t>555555555555</t>
-  </si>
-  <si>
     <t>380676556668</t>
   </si>
   <si>
@@ -148,9 +139,6 @@
     <t>380995111111</t>
   </si>
   <si>
-    <t>222223333333</t>
-  </si>
-  <si>
     <t>Андрій</t>
   </si>
   <si>
@@ -166,12 +154,6 @@
     <t>2005-03-05</t>
   </si>
   <si>
-    <t>444447777777</t>
-  </si>
-  <si>
-    <t>555555987654</t>
-  </si>
-  <si>
     <t>Дмитро</t>
   </si>
   <si>
@@ -190,24 +172,12 @@
     <t>1979-02-05</t>
   </si>
   <si>
-    <t>123438459832</t>
-  </si>
-  <si>
     <t>380678297656</t>
   </si>
   <si>
     <t>380989111333</t>
   </si>
   <si>
-    <t>333333320098</t>
-  </si>
-  <si>
-    <t>488829844444</t>
-  </si>
-  <si>
-    <t>555998055555</t>
-  </si>
-  <si>
     <t>380676753668</t>
   </si>
   <si>
@@ -217,13 +187,43 @@
     <t>380887711111</t>
   </si>
   <si>
-    <t>222229933333</t>
-  </si>
-  <si>
-    <t>447777777777</t>
-  </si>
-  <si>
-    <t>555553437654</t>
+    <t>380444444444</t>
+  </si>
+  <si>
+    <t>380555555555</t>
+  </si>
+  <si>
+    <t>380223333333</t>
+  </si>
+  <si>
+    <t>380447777777</t>
+  </si>
+  <si>
+    <t>380555987654</t>
+  </si>
+  <si>
+    <t>380438459832</t>
+  </si>
+  <si>
+    <t>380829844444</t>
+  </si>
+  <si>
+    <t>380333320098</t>
+  </si>
+  <si>
+    <t>380998055555</t>
+  </si>
+  <si>
+    <t>380229933333</t>
+  </si>
+  <si>
+    <t>380777777777</t>
+  </si>
+  <si>
+    <t>380553437654</t>
+  </si>
+  <si>
+    <t>380333333333</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -686,7 +686,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -755,10 +755,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -767,7 +767,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>17</v>
@@ -778,16 +778,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>29</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>24</v>
@@ -813,7 +813,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>19</v>
@@ -824,19 +824,19 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>17</v>
@@ -847,19 +847,19 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>18</v>
@@ -870,19 +870,19 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>19</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>24</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
@@ -1031,10 +1031,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1043,7 +1043,7 @@
         <v>23</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>17</v>
@@ -1054,16 +1054,16 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>29</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>24</v>
@@ -1089,7 +1089,7 @@
         <v>25</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>19</v>
@@ -1100,19 +1100,19 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>17</v>
@@ -1123,19 +1123,19 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>18</v>
@@ -1146,19 +1146,19 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Revert "update fetchUser and mailing-list"
This reverts commit 2d827745cf8be0e44bb377dbefbda835473fe7d3.
</commit_message>
<xml_diff>
--- a/public/contact_group_2.xlsx
+++ b/public/contact_group_2.xlsx
@@ -115,6 +115,15 @@
     <t>380995111333</t>
   </si>
   <si>
+    <t>333333333333</t>
+  </si>
+  <si>
+    <t>444444444444</t>
+  </si>
+  <si>
+    <t>555555555555</t>
+  </si>
+  <si>
     <t>380676556668</t>
   </si>
   <si>
@@ -139,6 +148,9 @@
     <t>380995111111</t>
   </si>
   <si>
+    <t>222223333333</t>
+  </si>
+  <si>
     <t>Андрій</t>
   </si>
   <si>
@@ -154,6 +166,12 @@
     <t>2005-03-05</t>
   </si>
   <si>
+    <t>444447777777</t>
+  </si>
+  <si>
+    <t>555555987654</t>
+  </si>
+  <si>
     <t>Дмитро</t>
   </si>
   <si>
@@ -172,12 +190,24 @@
     <t>1979-02-05</t>
   </si>
   <si>
+    <t>123438459832</t>
+  </si>
+  <si>
     <t>380678297656</t>
   </si>
   <si>
     <t>380989111333</t>
   </si>
   <si>
+    <t>333333320098</t>
+  </si>
+  <si>
+    <t>488829844444</t>
+  </si>
+  <si>
+    <t>555998055555</t>
+  </si>
+  <si>
     <t>380676753668</t>
   </si>
   <si>
@@ -187,43 +217,13 @@
     <t>380887711111</t>
   </si>
   <si>
-    <t>380444444444</t>
-  </si>
-  <si>
-    <t>380555555555</t>
-  </si>
-  <si>
-    <t>380223333333</t>
-  </si>
-  <si>
-    <t>380447777777</t>
-  </si>
-  <si>
-    <t>380555987654</t>
-  </si>
-  <si>
-    <t>380438459832</t>
-  </si>
-  <si>
-    <t>380829844444</t>
-  </si>
-  <si>
-    <t>380333320098</t>
-  </si>
-  <si>
-    <t>380998055555</t>
-  </si>
-  <si>
-    <t>380229933333</t>
-  </si>
-  <si>
-    <t>380777777777</t>
-  </si>
-  <si>
-    <t>380553437654</t>
-  </si>
-  <si>
-    <t>380333333333</t>
+    <t>222229933333</t>
+  </si>
+  <si>
+    <t>447777777777</t>
+  </si>
+  <si>
+    <t>555553437654</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -686,7 +686,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -755,10 +755,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -767,7 +767,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>17</v>
@@ -778,16 +778,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>29</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>24</v>
@@ -813,7 +813,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>19</v>
@@ -824,19 +824,19 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>17</v>
@@ -847,19 +847,19 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>18</v>
@@ -870,19 +870,19 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>19</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>24</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
@@ -1031,10 +1031,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1043,7 +1043,7 @@
         <v>23</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>17</v>
@@ -1054,16 +1054,16 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="4" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>29</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>24</v>
@@ -1089,7 +1089,7 @@
         <v>25</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>19</v>
@@ -1100,19 +1100,19 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>17</v>
@@ -1123,19 +1123,19 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>18</v>
@@ -1146,19 +1146,19 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>19</v>

</xml_diff>